<commit_message>
Removed finAll from stochastic
</commit_message>
<xml_diff>
--- a/Code/Optimiser/Stoc SolCheck.xlsx
+++ b/Code/Optimiser/Stoc SolCheck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Code\Optimiser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28FEC6D-9280-4050-B4F5-BB05B2DD9021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B601B48C-D3B3-493D-BDD8-A89CEDBB62C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C2CF203-BE44-4091-AD19-7EBDAA122E1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9C2CF203-BE44-4091-AD19-7EBDAA122E1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +218,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -231,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -244,6 +256,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A32A4A6-99F3-4C76-86D2-7F74D01F6745}">
   <dimension ref="A1:CM53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG14" sqref="AG14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AG3" sqref="AG3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,14 +745,14 @@
         <v>4</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:AL6" si="0">H3+$A$5</f>
+        <f t="shared" ref="N3:AF6" si="0">H3+$A$5</f>
         <v>8</v>
       </c>
       <c r="T3" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="12">
         <v>2</v>
       </c>
       <c r="Z3" s="4">
@@ -762,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H18" si="2">B4+$A$5</f>
+        <f t="shared" ref="H4:H6" si="2">B4+$A$5</f>
         <v>5</v>
       </c>
       <c r="N4" s="4">
@@ -805,9 +819,6 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="U5" s="4">
-        <v>1</v>
-      </c>
       <c r="Z5" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -837,8 +848,8 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="U6" s="4">
-        <v>1</v>
+      <c r="V6" s="12">
+        <v>2</v>
       </c>
       <c r="Z6" s="4">
         <f t="shared" si="0"/>
@@ -996,8 +1007,8 @@
         <f>AF3+A5</f>
         <v>24</v>
       </c>
-      <c r="C11" s="4">
-        <v>4</v>
+      <c r="D11" s="13">
+        <v>1</v>
       </c>
       <c r="H11" s="4">
         <f>B11+$A$5</f>
@@ -1011,12 +1022,12 @@
         <f>N11+$A$5</f>
         <v>36</v>
       </c>
+      <c r="V11" s="13">
+        <v>0</v>
+      </c>
       <c r="Z11" s="4">
         <f>T11+$A$5</f>
         <v>40</v>
-      </c>
-      <c r="AA11" s="4">
-        <v>3</v>
       </c>
       <c r="AF11" s="4">
         <f>Z11+$A$5</f>
@@ -1033,6 +1044,9 @@
         <f>B11+1</f>
         <v>25</v>
       </c>
+      <c r="D12" s="13">
+        <v>1</v>
+      </c>
       <c r="H12" s="4">
         <f>B12+$A$5</f>
         <v>29</v>
@@ -1044,6 +1058,9 @@
       <c r="T12" s="4">
         <f>N12+$A$5</f>
         <v>37</v>
+      </c>
+      <c r="V12" s="13">
+        <v>0</v>
       </c>
       <c r="W12" s="11"/>
       <c r="Z12" s="4">
@@ -1064,7 +1081,7 @@
         <f t="shared" ref="B13:B14" si="3">B12+1</f>
         <v>26</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="13">
         <v>0</v>
       </c>
       <c r="H13" s="4">
@@ -1079,6 +1096,9 @@
         <f>N13+$A$5</f>
         <v>38</v>
       </c>
+      <c r="U13" s="13">
+        <v>1</v>
+      </c>
       <c r="Z13" s="4">
         <f>T13+$A$5</f>
         <v>42</v>
@@ -1097,7 +1117,7 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="13">
         <v>0</v>
       </c>
       <c r="H14" s="4">
@@ -1111,6 +1131,9 @@
       <c r="T14" s="4">
         <f>N14+$A$5</f>
         <v>39</v>
+      </c>
+      <c r="U14" s="13">
+        <v>1</v>
       </c>
       <c r="Z14" s="4">
         <f>T14+$A$5</f>
@@ -2056,8 +2079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C642237E-D03A-45EC-B312-ECA8F260C28A}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,7 +2101,7 @@
       </c>
       <c r="F1">
         <f>SUM(G21:G68) - SUM(G6:G17)</f>
-        <v>148.23675408900817</v>
+        <v>15376.836816908315</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2125,7 +2148,7 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <f>POWER($B$3, A6)</f>
+        <f t="shared" ref="B6:B17" si="0">POWER($B$3, A6)</f>
         <v>1</v>
       </c>
       <c r="C6">
@@ -2135,7 +2158,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <f>C6*$B$2+D6*$C$2</f>
+        <f t="shared" ref="E6:E17" si="1">C6*$B$2+D6*$C$2</f>
         <v>0</v>
       </c>
       <c r="G6">
@@ -2148,7 +2171,7 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <f>POWER($B$3, A7)</f>
+        <f t="shared" si="0"/>
         <v>0.99916280000000002</v>
       </c>
       <c r="C7">
@@ -2158,11 +2181,11 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <f>C7*$B$2+D7*$C$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G17" si="0">B7*E7</f>
+        <f t="shared" ref="G7:G17" si="2">B7*E7</f>
         <v>0</v>
       </c>
     </row>
@@ -2171,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <f>POWER($B$3, A8)</f>
+        <f t="shared" si="0"/>
         <v>0.99832630090384</v>
       </c>
       <c r="C8">
@@ -2181,11 +2204,11 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <f>C8*$B$2+D8*$C$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2194,22 +2217,22 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <f>POWER($B$3, A9)</f>
+        <f t="shared" si="0"/>
         <v>0.99749050212472334</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <f>C9*$B$2+D9*$C$2</f>
-        <v>5500</v>
+        <f t="shared" si="1"/>
+        <v>3500</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
-        <v>5486.1977616859785</v>
+        <f t="shared" si="2"/>
+        <v>3491.2167574365317</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2217,7 +2240,7 @@
         <v>4</v>
       </c>
       <c r="B10">
-        <f>POWER($B$3, A10)</f>
+        <f t="shared" si="0"/>
         <v>0.99665540307634448</v>
       </c>
       <c r="C10">
@@ -2227,11 +2250,11 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <f>C10*$B$2+D10*$C$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2240,7 +2263,7 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <f>POWER($B$3, A11)</f>
+        <f t="shared" si="0"/>
         <v>0.99582100317288902</v>
       </c>
       <c r="C11">
@@ -2250,11 +2273,11 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <f>C11*$B$2+D11*$C$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2263,7 +2286,7 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <f>POWER($B$3, A12)</f>
+        <f t="shared" si="0"/>
         <v>0.99498730182903261</v>
       </c>
       <c r="C12">
@@ -2273,11 +2296,11 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <f>C12*$B$2+D12*$C$2</f>
+        <f t="shared" si="1"/>
         <v>5500</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5472.4301600596791</v>
       </c>
     </row>
@@ -2286,7 +2309,7 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <f>POWER($B$3, A13)</f>
+        <f t="shared" si="0"/>
         <v>0.99415429845994141</v>
       </c>
       <c r="C13">
@@ -2296,11 +2319,11 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <f>C13*$B$2+D13*$C$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2309,7 +2332,7 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <f>POWER($B$3, A14)</f>
+        <f t="shared" si="0"/>
         <v>0.99332199248127073</v>
       </c>
       <c r="C14">
@@ -2319,11 +2342,11 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <f>C14*$B$2+D14*$C$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2332,22 +2355,22 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <f>POWER($B$3, A15)</f>
+        <f t="shared" si="0"/>
         <v>0.99249038330916539</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <f>C15*$B$2+D15*$C$2</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5500</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>5458.6971082004093</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2355,22 +2378,22 @@
         <v>10</v>
       </c>
       <c r="B16">
-        <f>POWER($B$3, A16)</f>
+        <f t="shared" si="0"/>
         <v>0.99165947036025903</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <f>C16*$B$2+D16*$C$2</f>
-        <v>3500</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
-        <v>3470.8081462609066</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -2378,7 +2401,7 @@
         <v>11</v>
       </c>
       <c r="B17">
-        <f>POWER($B$3, A17)</f>
+        <f t="shared" si="0"/>
         <v>0.99082925305167346</v>
       </c>
       <c r="C17">
@@ -2388,11 +2411,11 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <f>C17*$B$2+D17*$C$2</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2452,11 +2475,11 @@
         <v>480</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21">
         <f>E21*D21*B21</f>
-        <v>480</v>
+        <v>960</v>
       </c>
       <c r="I21">
         <v>400</v>
@@ -2470,7 +2493,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" ref="A22:A68" si="1">_xlfn.FLOOR.MATH(C22/$B$1)</f>
+        <f t="shared" ref="A22:A68" si="3">_xlfn.FLOOR.MATH(C22/$B$1)</f>
         <v>0</v>
       </c>
       <c r="B22">
@@ -2481,15 +2504,15 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:D68" si="2">AVERAGE(I22:K22)</f>
+        <f t="shared" ref="D22:D68" si="4">AVERAGE(I22:K22)</f>
         <v>480</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <f t="shared" ref="G22:G68" si="3">E22*D22*B22</f>
-        <v>480</v>
+        <f t="shared" ref="G22:G68" si="5">E22*D22*B22</f>
+        <v>960</v>
       </c>
       <c r="I22">
         <v>400</v>
@@ -2503,26 +2526,26 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:B68" si="4">B22</f>
+        <f t="shared" ref="B23:B24" si="6">B22</f>
         <v>1</v>
       </c>
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
-        <v>480</v>
+        <f t="shared" si="5"/>
+        <v>960</v>
       </c>
       <c r="I23">
         <v>400</v>
@@ -2536,26 +2559,26 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="B24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
-        <v>480</v>
+        <f t="shared" si="5"/>
+        <v>960</v>
       </c>
       <c r="I24">
         <v>400</v>
@@ -2569,7 +2592,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B25">
@@ -2580,15 +2603,15 @@
         <v>4</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
-        <v>479.59814399999999</v>
+        <f t="shared" si="5"/>
+        <v>959.19628799999998</v>
       </c>
       <c r="I25">
         <v>400</v>
@@ -2602,26 +2625,26 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:B68" si="5">B22*$B$3</f>
+        <f t="shared" ref="B26:B68" si="7">B22*$B$3</f>
         <v>0.99916280000000002</v>
       </c>
       <c r="C26">
         <v>5</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
-        <v>479.59814399999999</v>
+        <f t="shared" si="5"/>
+        <v>959.19628799999998</v>
       </c>
       <c r="I26">
         <v>400</v>
@@ -2635,26 +2658,26 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99916280000000002</v>
       </c>
       <c r="C27">
         <v>6</v>
       </c>
       <c r="D27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
-        <v>479.59814399999999</v>
+        <f t="shared" si="5"/>
+        <v>959.19628799999998</v>
       </c>
       <c r="I27">
         <v>400</v>
@@ -2668,26 +2691,26 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="B28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99916280000000002</v>
       </c>
       <c r="C28">
         <v>7</v>
       </c>
       <c r="D28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
-        <v>479.59814399999999</v>
+        <f t="shared" si="5"/>
+        <v>959.19628799999998</v>
       </c>
       <c r="I28">
         <v>400</v>
@@ -2701,26 +2724,26 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="B29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99832630090384</v>
       </c>
       <c r="C29">
         <v>8</v>
       </c>
       <c r="D29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <f t="shared" si="3"/>
-        <v>479.19662443384323</v>
+        <f t="shared" si="5"/>
+        <v>958.39324886768645</v>
       </c>
       <c r="I29">
         <v>400</v>
@@ -2734,26 +2757,26 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="B30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99832630090384</v>
       </c>
       <c r="C30">
         <v>9</v>
       </c>
       <c r="D30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30">
-        <f t="shared" si="3"/>
-        <v>479.19662443384323</v>
+        <f t="shared" si="5"/>
+        <v>958.39324886768645</v>
       </c>
       <c r="I30">
         <v>400</v>
@@ -2767,26 +2790,26 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="B31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99832630090384</v>
       </c>
       <c r="C31">
         <v>10</v>
       </c>
       <c r="D31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G31">
-        <f t="shared" si="3"/>
-        <v>479.19662443384323</v>
+        <f t="shared" si="5"/>
+        <v>958.39324886768645</v>
       </c>
       <c r="I31">
         <v>400</v>
@@ -2800,26 +2823,26 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="B32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99832630090384</v>
       </c>
       <c r="C32">
         <v>11</v>
       </c>
       <c r="D32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
-        <v>479.19662443384323</v>
+        <f t="shared" si="5"/>
+        <v>958.39324886768645</v>
       </c>
       <c r="I32">
         <v>400</v>
@@ -2833,26 +2856,26 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99749050212472334</v>
       </c>
       <c r="C33">
         <v>12</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>478.79544101986721</v>
       </c>
       <c r="I33">
         <v>400</v>
@@ -2866,26 +2889,26 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99749050212472334</v>
       </c>
       <c r="C34">
         <v>13</v>
       </c>
       <c r="D34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G34">
-        <f t="shared" si="3"/>
-        <v>478.79544101986721</v>
+        <f t="shared" si="5"/>
+        <v>957.59088203973442</v>
       </c>
       <c r="I34">
         <v>400</v>
@@ -2899,26 +2922,26 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99749050212472334</v>
       </c>
       <c r="C35">
         <v>14</v>
       </c>
       <c r="D35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>480</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G35">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>957.59088203973442</v>
       </c>
       <c r="I35">
         <v>400</v>
@@ -2932,26 +2955,26 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="B36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99749050212472334</v>
       </c>
       <c r="C36">
         <v>15</v>
       </c>
       <c r="D36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>265.99746723325956</v>
       </c>
       <c r="I36">
         <v>400</v>
@@ -2965,26 +2988,26 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99665540307634459</v>
       </c>
       <c r="C37">
         <v>16</v>
       </c>
       <c r="D37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G37">
-        <f t="shared" si="3"/>
-        <v>265.77477415369191</v>
+        <f t="shared" si="5"/>
+        <v>531.54954830738382</v>
       </c>
       <c r="I37">
         <v>400</v>
@@ -2998,26 +3021,26 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99665540307634459</v>
       </c>
       <c r="C38">
         <v>17</v>
       </c>
       <c r="D38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G38">
-        <f t="shared" si="3"/>
-        <v>265.77477415369191</v>
+        <f t="shared" si="5"/>
+        <v>531.54954830738382</v>
       </c>
       <c r="I38">
         <v>400</v>
@@ -3031,26 +3054,26 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99665540307634459</v>
       </c>
       <c r="C39">
         <v>18</v>
       </c>
       <c r="D39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G39">
-        <f t="shared" si="3"/>
-        <v>265.77477415369191</v>
+        <f t="shared" si="5"/>
+        <v>531.54954830738382</v>
       </c>
       <c r="I39">
         <v>400</v>
@@ -3064,26 +3087,26 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="B40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99665540307634459</v>
       </c>
       <c r="C40">
         <v>19</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G40">
-        <f t="shared" si="3"/>
-        <v>265.77477415369191</v>
+        <f t="shared" si="5"/>
+        <v>531.54954830738382</v>
       </c>
       <c r="I40">
         <v>400</v>
@@ -3097,25 +3120,25 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99582100317288913</v>
       </c>
       <c r="C41">
         <v>20</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="G41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>265.55226751277047</v>
       </c>
       <c r="I41">
@@ -3130,25 +3153,25 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99582100317288913</v>
       </c>
       <c r="C42">
         <v>21</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
       <c r="G42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>265.55226751277047</v>
       </c>
       <c r="I42">
@@ -3163,26 +3186,26 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99582100317288913</v>
       </c>
       <c r="C43">
         <v>22</v>
       </c>
       <c r="D43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>265.55226751277047</v>
       </c>
       <c r="I43">
         <v>400</v>
@@ -3196,25 +3219,25 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="B44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99582100317288913</v>
       </c>
       <c r="C44">
         <v>23</v>
       </c>
       <c r="D44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="G44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I44">
@@ -3229,25 +3252,25 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99498730182903283</v>
       </c>
       <c r="C45">
         <v>24</v>
       </c>
       <c r="D45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="G45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I45">
@@ -3262,26 +3285,26 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99498730182903283</v>
       </c>
       <c r="C46">
         <v>25</v>
       </c>
       <c r="D46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <f t="shared" si="3"/>
-        <v>265.32994715440879</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="I46">
         <v>400</v>
@@ -3295,26 +3318,26 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99498730182903283</v>
       </c>
       <c r="C47">
         <v>26</v>
       </c>
       <c r="D47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>265.32994715440879</v>
       </c>
       <c r="I47">
         <v>400</v>
@@ -3328,26 +3351,26 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="B48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99498730182903283</v>
       </c>
       <c r="C48">
         <v>27</v>
       </c>
       <c r="D48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>265.32994715440879</v>
       </c>
       <c r="I48">
         <v>400</v>
@@ -3361,26 +3384,26 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99415429845994163</v>
       </c>
       <c r="C49">
         <v>28</v>
       </c>
       <c r="D49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G49">
-        <f t="shared" si="3"/>
-        <v>265.10781292265114</v>
+        <f t="shared" si="5"/>
+        <v>530.21562584530227</v>
       </c>
       <c r="I49">
         <v>400</v>
@@ -3394,26 +3417,26 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99415429845994163</v>
       </c>
       <c r="C50">
         <v>29</v>
       </c>
       <c r="D50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>266.66666666666669</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <f t="shared" si="3"/>
-        <v>265.10781292265114</v>
+        <f t="shared" si="5"/>
+        <v>530.21562584530227</v>
       </c>
       <c r="I50">
         <v>400</v>
@@ -3427,26 +3450,26 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99415429845994163</v>
       </c>
       <c r="C51">
         <v>30</v>
       </c>
       <c r="D51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G51">
-        <f t="shared" si="3"/>
-        <v>397.66171938397667</v>
+        <f t="shared" si="5"/>
+        <v>795.32343876795335</v>
       </c>
       <c r="I51">
         <v>400</v>
@@ -3460,26 +3483,26 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="B52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99415429845994163</v>
       </c>
       <c r="C52">
         <v>31</v>
       </c>
       <c r="D52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G52">
-        <f t="shared" si="3"/>
-        <v>397.66171938397667</v>
+        <f t="shared" si="5"/>
+        <v>795.32343876795335</v>
       </c>
       <c r="I52">
         <v>400</v>
@@ -3493,26 +3516,26 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99332199248127095</v>
       </c>
       <c r="C53">
         <v>32</v>
       </c>
       <c r="D53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G53">
-        <f t="shared" si="3"/>
-        <v>397.32879699250839</v>
+        <f t="shared" si="5"/>
+        <v>794.65759398501677</v>
       </c>
       <c r="I53">
         <v>400</v>
@@ -3526,26 +3549,26 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99332199248127095</v>
       </c>
       <c r="C54">
         <v>33</v>
       </c>
       <c r="D54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G54">
-        <f t="shared" si="3"/>
-        <v>397.32879699250839</v>
+        <f t="shared" si="5"/>
+        <v>794.65759398501677</v>
       </c>
       <c r="I54">
         <v>400</v>
@@ -3559,26 +3582,26 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99332199248127095</v>
       </c>
       <c r="C55">
         <v>34</v>
       </c>
       <c r="D55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G55">
-        <f t="shared" si="3"/>
-        <v>397.32879699250839</v>
+        <f t="shared" si="5"/>
+        <v>794.65759398501677</v>
       </c>
       <c r="I55">
         <v>400</v>
@@ -3592,25 +3615,25 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="B56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99332199248127095</v>
       </c>
       <c r="C56">
         <v>35</v>
       </c>
       <c r="D56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="G56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>397.32879699250839</v>
       </c>
       <c r="I56">
@@ -3625,25 +3648,25 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99249038330916561</v>
       </c>
       <c r="C57">
         <v>36</v>
       </c>
       <c r="D57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E57">
         <v>1</v>
       </c>
       <c r="G57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>396.99615332366625</v>
       </c>
       <c r="I57">
@@ -3658,25 +3681,25 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99249038330916561</v>
       </c>
       <c r="C58">
         <v>37</v>
       </c>
       <c r="D58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
       <c r="G58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>396.99615332366625</v>
       </c>
       <c r="I58">
@@ -3691,26 +3714,26 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99249038330916561</v>
       </c>
       <c r="C59">
         <v>38</v>
       </c>
       <c r="D59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>396.99615332366625</v>
       </c>
       <c r="I59">
         <v>400</v>
@@ -3724,26 +3747,26 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="B60">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99249038330916561</v>
       </c>
       <c r="C60">
         <v>39</v>
       </c>
       <c r="D60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>396.99615332366625</v>
       </c>
       <c r="I60">
         <v>400</v>
@@ -3757,26 +3780,26 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B61">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99165947036025914</v>
       </c>
       <c r="C61">
         <v>40</v>
       </c>
       <c r="D61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G61">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>793.3275762882073</v>
       </c>
       <c r="I61">
         <v>400</v>
@@ -3790,26 +3813,26 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99165947036025914</v>
       </c>
       <c r="C62">
         <v>41</v>
       </c>
       <c r="D62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G62">
-        <f t="shared" si="3"/>
-        <v>396.66378814410365</v>
+        <f t="shared" si="5"/>
+        <v>793.3275762882073</v>
       </c>
       <c r="I62">
         <v>400</v>
@@ -3823,26 +3846,26 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B63">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99165947036025914</v>
       </c>
       <c r="C63">
         <v>42</v>
       </c>
       <c r="D63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63">
-        <f t="shared" si="3"/>
-        <v>396.66378814410365</v>
+        <f t="shared" si="5"/>
+        <v>793.3275762882073</v>
       </c>
       <c r="I63">
         <v>400</v>
@@ -3856,26 +3879,26 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="B64">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99165947036025914</v>
       </c>
       <c r="C64">
         <v>43</v>
       </c>
       <c r="D64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G64">
-        <f t="shared" si="3"/>
-        <v>396.66378814410365</v>
+        <f t="shared" si="5"/>
+        <v>793.3275762882073</v>
       </c>
       <c r="I64">
         <v>400</v>
@@ -3889,26 +3912,26 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99082925305167358</v>
       </c>
       <c r="C65">
         <v>44</v>
       </c>
       <c r="D65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65">
-        <f t="shared" si="3"/>
-        <v>396.3317012206694</v>
+        <f t="shared" si="5"/>
+        <v>792.6634024413388</v>
       </c>
       <c r="I65">
         <v>400</v>
@@ -3922,26 +3945,26 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B66">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99082925305167358</v>
       </c>
       <c r="C66">
         <v>45</v>
       </c>
       <c r="D66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G66">
-        <f t="shared" si="3"/>
-        <v>396.3317012206694</v>
+        <f t="shared" si="5"/>
+        <v>792.6634024413388</v>
       </c>
       <c r="I66">
         <v>400</v>
@@ -3955,25 +3978,25 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B67">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99082925305167358</v>
       </c>
       <c r="C67">
         <v>46</v>
       </c>
       <c r="D67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E67">
         <v>1</v>
       </c>
       <c r="G67">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>396.3317012206694</v>
       </c>
       <c r="I67">
@@ -3988,26 +4011,26 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="B68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.99082925305167358</v>
       </c>
       <c r="C68">
         <v>47</v>
       </c>
       <c r="D68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <f t="shared" si="3"/>
-        <v>396.3317012206694</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="I68">
         <v>400</v>

</xml_diff>